<commit_message>
updated the PC naming function to use the high and low prompts explicitly (rather than value dimensions)
</commit_message>
<xml_diff>
--- a/example data/EXAMPLE_scale-definitions_multi_MHON.xlsx
+++ b/example data/EXAMPLE_scale-definitions_multi_MHON.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Dropbox\python-projects\compost-tp\github docs\example data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\value-dimension-analysis-for-design-process\example data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6555AB36-AD4F-4FDB-AA52-9406DAC49677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C68453-100A-4BAD-88DC-BF1D9F69D04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5484" yWindow="2064" windowWidth="17592" windowHeight="8892" xr2:uid="{42D28C09-D715-4881-9C3E-C3FC8B40E215}"/>
+    <workbookView xWindow="1740" yWindow="855" windowWidth="24900" windowHeight="13995" xr2:uid="{42D28C09-D715-4881-9C3E-C3FC8B40E215}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>scale_point</t>
   </si>
   <si>
-    <t>lowest potential for addressing the respective sustainable development goal</t>
-  </si>
-  <si>
     <t>Physiological needs</t>
   </si>
   <si>
@@ -66,6 +63,12 @@
   </si>
   <si>
     <t>Transcendence needs</t>
+  </si>
+  <si>
+    <t>highest potential for addressing the respective need</t>
+  </si>
+  <si>
+    <t>lowest potential for addressing the respective need</t>
   </si>
 </sst>
 </file>
@@ -449,43 +452,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D99CCC-ED7B-4B10-9AD9-B2906C78E768}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -497,33 +500,33 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -535,7 +538,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -557,7 +560,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -579,7 +582,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -601,33 +604,33 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>

</xml_diff>